<commit_message>
Sankey add grouping. Move files to test folder.
</commit_message>
<xml_diff>
--- a/data/sankey/sankey.xlsx
+++ b/data/sankey/sankey.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\An\Documents\GitHub\COS30045\data\sankey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF5FD90-3356-4271-A588-B41DFA9FEFB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC38D18-0FA1-4610-9888-C3DF778D33FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="230">
   <si>
     <t>MSN</t>
   </si>
@@ -731,6 +731,9 @@
   </si>
   <si>
     <t>#F0ECE2</t>
+  </si>
+  <si>
+    <t>pink</t>
   </si>
 </sst>
 </file>
@@ -1604,8 +1607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD520A74-6D21-4711-8177-C48F7CF78287}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2160,6 +2163,9 @@
       <c r="E28">
         <v>2</v>
       </c>
+      <c r="F28" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
@@ -2176,6 +2182,9 @@
       </c>
       <c r="E29">
         <v>4</v>
+      </c>
+      <c r="F29" t="s">
+        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -4103,7 +4112,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A13" sqref="A1:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4288,7 +4297,7 @@
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>211</v>
+        <v>229</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>